<commit_message>
Proxies updated to 2019:6
</commit_message>
<xml_diff>
--- a/ff4_instruments_shared.xlsx
+++ b/ff4_instruments_shared.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Projects\IV Extension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\osiride-fs\m035315\private\Code\MAR_update_2019\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E4097B-17A0-43E0-9F82-3C9FC213FD9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7125"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ver_2025" sheetId="2" r:id="rId1"/>
+    <sheet name="ver_2024" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Time</t>
   </si>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -67,9 +69,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -349,15 +352,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C337"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A032EFC-B956-4033-BA98-9ECF3E30E3B6}">
+  <dimension ref="A1:C343"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="3" width="16.42578125" customWidth="1"/>
+    <col min="1" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -372,6 +374,3795 @@
       </c>
     </row>
     <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>33239</v>
+      </c>
+      <c r="B2">
+        <v>1.2211783271134161E-3</v>
+      </c>
+      <c r="C2">
+        <v>5.8420658241109535E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>33270</v>
+      </c>
+      <c r="B3">
+        <v>-4.4038163438161256E-2</v>
+      </c>
+      <c r="C3">
+        <v>-7.6437048000312785E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>33298</v>
+      </c>
+      <c r="B4">
+        <v>6.8021571732809538E-2</v>
+      </c>
+      <c r="C4">
+        <v>-2.9693579539163503E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>33329</v>
+      </c>
+      <c r="B5">
+        <v>-0.11814868725263956</v>
+      </c>
+      <c r="C5">
+        <v>3.0317677915044632E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>33359</v>
+      </c>
+      <c r="B6">
+        <v>2.7383198108409813E-2</v>
+      </c>
+      <c r="C6">
+        <v>4.4775784408385463E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>33390</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
+        <v>33420</v>
+      </c>
+      <c r="B8">
+        <v>4.1961771604352244E-2</v>
+      </c>
+      <c r="C8">
+        <v>1.8341740798824082E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
+        <v>33451</v>
+      </c>
+      <c r="B9">
+        <v>1.7104866323730331E-3</v>
+      </c>
+      <c r="C9">
+        <v>-2.4725413422246299E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2">
+        <v>33482</v>
+      </c>
+      <c r="B10">
+        <v>7.5976375663700949E-3</v>
+      </c>
+      <c r="C10">
+        <v>3.4958761781410393E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2">
+        <v>33512</v>
+      </c>
+      <c r="B11">
+        <v>1.3160421892885184E-2</v>
+      </c>
+      <c r="C11">
+        <v>-1.1121137854854246E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2">
+        <v>33543</v>
+      </c>
+      <c r="B12">
+        <v>-7.1432809467590827E-2</v>
+      </c>
+      <c r="C12">
+        <v>1.0520060986827305E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2">
+        <v>33573</v>
+      </c>
+      <c r="B13">
+        <v>-9.9527657743116477E-2</v>
+      </c>
+      <c r="C13">
+        <v>-5.7254562728042122E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2">
+        <v>33604</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2">
+        <v>33635</v>
+      </c>
+      <c r="B15">
+        <v>2.9781642344939754E-2</v>
+      </c>
+      <c r="C15">
+        <v>2.1654860289033129E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2">
+        <v>33664</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2">
+        <v>33695</v>
+      </c>
+      <c r="B17">
+        <v>-0.14144262437196242</v>
+      </c>
+      <c r="C17">
+        <v>-1.5862424045034657E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2">
+        <v>33725</v>
+      </c>
+      <c r="B18">
+        <v>1.1304853126734783E-2</v>
+      </c>
+      <c r="C18">
+        <v>9.2578537124905491E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2">
+        <v>33756</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2">
+        <v>33786</v>
+      </c>
+      <c r="B20">
+        <v>-0.23657884040106547</v>
+      </c>
+      <c r="C20">
+        <v>2.1667700134937497E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2">
+        <v>33817</v>
+      </c>
+      <c r="B21">
+        <v>-1.7836715098275904E-2</v>
+      </c>
+      <c r="C21">
+        <v>-6.4035549382909264E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2">
+        <v>33848</v>
+      </c>
+      <c r="B22">
+        <v>-3.4849131238750899E-2</v>
+      </c>
+      <c r="C22">
+        <v>1.5239981259514037E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2">
+        <v>33878</v>
+      </c>
+      <c r="B23">
+        <v>5.2371985814964009E-2</v>
+      </c>
+      <c r="C23">
+        <v>-9.5305879009072204E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2">
+        <v>33909</v>
+      </c>
+      <c r="B24">
+        <v>4.8739768047773899E-2</v>
+      </c>
+      <c r="C24">
+        <v>9.3566018126759673E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2">
+        <v>33939</v>
+      </c>
+      <c r="B25">
+        <v>-8.0254704717842278E-3</v>
+      </c>
+      <c r="C25">
+        <v>3.3800001910630609E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2">
+        <v>33970</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2">
+        <v>34001</v>
+      </c>
+      <c r="B27">
+        <v>2.7146469724994023E-2</v>
+      </c>
+      <c r="C27">
+        <v>-1.3365787035674788E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2">
+        <v>34029</v>
+      </c>
+      <c r="B28">
+        <v>1.4270734042201159E-2</v>
+      </c>
+      <c r="C28">
+        <v>-4.9556935675986215E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2">
+        <v>34060</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2">
+        <v>34090</v>
+      </c>
+      <c r="B30">
+        <v>1.3344118189009886E-2</v>
+      </c>
+      <c r="C30">
+        <v>-7.7364591933973895E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2">
+        <v>34121</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2">
+        <v>34151</v>
+      </c>
+      <c r="B32">
+        <v>4.9009504160453521E-4</v>
+      </c>
+      <c r="C32">
+        <v>8.1551294953801281E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2">
+        <v>34182</v>
+      </c>
+      <c r="B33">
+        <v>1.9791753635645254E-2</v>
+      </c>
+      <c r="C33">
+        <v>-4.6866059752648914E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2">
+        <v>34213</v>
+      </c>
+      <c r="B34">
+        <v>3.9460897650866036E-2</v>
+      </c>
+      <c r="C34">
+        <v>-1.2737190712407247E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2">
+        <v>34243</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2">
+        <v>34274</v>
+      </c>
+      <c r="B36">
+        <v>1.5751911328088456E-3</v>
+      </c>
+      <c r="C36">
+        <v>2.228733095375135E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2">
+        <v>34304</v>
+      </c>
+      <c r="B37">
+        <v>-3.0597853711426152E-2</v>
+      </c>
+      <c r="C37">
+        <v>1.6173248286088938E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2">
+        <v>34335</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2">
+        <v>34366</v>
+      </c>
+      <c r="B39">
+        <v>-3.3035883359157837E-2</v>
+      </c>
+      <c r="C39">
+        <v>-3.3690097630027734E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2">
+        <v>34394</v>
+      </c>
+      <c r="B40">
+        <v>-1.1005209784838295E-2</v>
+      </c>
+      <c r="C40">
+        <v>-2.0512341232492778E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2">
+        <v>34425</v>
+      </c>
+      <c r="B41">
+        <v>0.11925752259075628</v>
+      </c>
+      <c r="C41">
+        <v>2.3011501377620189E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2">
+        <v>34455</v>
+      </c>
+      <c r="B42">
+        <v>4.9750251457437403E-2</v>
+      </c>
+      <c r="C42">
+        <v>2.2847733030130643E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2">
+        <v>34486</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="2">
+        <v>34516</v>
+      </c>
+      <c r="B44">
+        <v>-1.684251782786467E-2</v>
+      </c>
+      <c r="C44">
+        <v>-1.0726027941947312E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="2">
+        <v>34547</v>
+      </c>
+      <c r="B45">
+        <v>-3.5926940281143412E-4</v>
+      </c>
+      <c r="C45">
+        <v>-1.0886529047547996E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2">
+        <v>34578</v>
+      </c>
+      <c r="B46">
+        <v>-5.2600580981238799E-2</v>
+      </c>
+      <c r="C46">
+        <v>1.0005819182797276E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2">
+        <v>34608</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2">
+        <v>34639</v>
+      </c>
+      <c r="B48">
+        <v>5.7941647360767325E-2</v>
+      </c>
+      <c r="C48">
+        <v>6.6524408236483638E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2">
+        <v>34669</v>
+      </c>
+      <c r="B49">
+        <v>-5.9500421150333299E-2</v>
+      </c>
+      <c r="C49">
+        <v>1.3523862318625172E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2">
+        <v>34700</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2">
+        <v>34731</v>
+      </c>
+      <c r="B51">
+        <v>-1.4597342304298083E-2</v>
+      </c>
+      <c r="C51">
+        <v>-2.257630291552189E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2">
+        <v>34759</v>
+      </c>
+      <c r="B52">
+        <v>3.0496894888948165E-2</v>
+      </c>
+      <c r="C52">
+        <v>-3.4918207233498935E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2">
+        <v>34790</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2">
+        <v>34820</v>
+      </c>
+      <c r="B54">
+        <v>3.1170276605152911E-2</v>
+      </c>
+      <c r="C54">
+        <v>-9.3488144913177994E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2">
+        <v>34851</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2">
+        <v>34881</v>
+      </c>
+      <c r="B56">
+        <v>-8.2201252013327536E-2</v>
+      </c>
+      <c r="C56">
+        <v>-3.1822835283871094E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2">
+        <v>34912</v>
+      </c>
+      <c r="B57">
+        <v>1.7211491383601122E-2</v>
+      </c>
+      <c r="C57">
+        <v>3.3701410462040979E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2">
+        <v>34943</v>
+      </c>
+      <c r="B58">
+        <v>8.9305260706503305E-3</v>
+      </c>
+      <c r="C58">
+        <v>2.3945085758865697E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="2">
+        <v>34973</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="2">
+        <v>35004</v>
+      </c>
+      <c r="B60">
+        <v>5.3225841806428836E-2</v>
+      </c>
+      <c r="C60">
+        <v>-1.2624256433012994E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2">
+        <v>35034</v>
+      </c>
+      <c r="B61">
+        <v>-3.3286969792379231E-2</v>
+      </c>
+      <c r="C61">
+        <v>-1.0962227886437057E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="2">
+        <v>35065</v>
+      </c>
+      <c r="B62">
+        <v>5.5061216299982447E-3</v>
+      </c>
+      <c r="C62">
+        <v>-5.5279592581318621E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2">
+        <v>35096</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="2">
+        <v>35125</v>
+      </c>
+      <c r="B64">
+        <v>1.7149868585510833E-2</v>
+      </c>
+      <c r="C64">
+        <v>4.73740712341136E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="2">
+        <v>35156</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2">
+        <v>35186</v>
+      </c>
+      <c r="B66">
+        <v>1.3921480134785998E-2</v>
+      </c>
+      <c r="C66">
+        <v>1.3402074283901687E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2">
+        <v>35217</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2">
+        <v>35247</v>
+      </c>
+      <c r="B68">
+        <v>-2.8094492325776779E-2</v>
+      </c>
+      <c r="C68">
+        <v>1.1842606703111706E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2">
+        <v>35278</v>
+      </c>
+      <c r="B69">
+        <v>1.9027286619421289E-2</v>
+      </c>
+      <c r="C69">
+        <v>-1.1179584256512803E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2">
+        <v>35309</v>
+      </c>
+      <c r="B70">
+        <v>-0.11799849353679044</v>
+      </c>
+      <c r="C70">
+        <v>-1.1257644787388629E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2">
+        <v>35339</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2">
+        <v>35370</v>
+      </c>
+      <c r="B72">
+        <v>-2.5349197159446144E-3</v>
+      </c>
+      <c r="C72">
+        <v>-1.5711627400290355E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2">
+        <v>35400</v>
+      </c>
+      <c r="B73">
+        <v>6.2631992061092266E-3</v>
+      </c>
+      <c r="C73">
+        <v>-1.4653199417012167E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2">
+        <v>35431</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="2">
+        <v>35462</v>
+      </c>
+      <c r="B75">
+        <v>1.8122758033570493E-2</v>
+      </c>
+      <c r="C75">
+        <v>-1.084012351672793E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="2">
+        <v>35490</v>
+      </c>
+      <c r="B76">
+        <v>6.2564205179256663E-2</v>
+      </c>
+      <c r="C76">
+        <v>-1.1355459215461675E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2">
+        <v>35521</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="2">
+        <v>35551</v>
+      </c>
+      <c r="B78">
+        <v>-2.6978302392426896E-2</v>
+      </c>
+      <c r="C78">
+        <v>-1.9745243586171687E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="2">
+        <v>35582</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="2">
+        <v>35612</v>
+      </c>
+      <c r="B80">
+        <v>-1.058928902651577E-2</v>
+      </c>
+      <c r="C80">
+        <v>-2.648119412323624E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2">
+        <v>35643</v>
+      </c>
+      <c r="B81">
+        <v>1.7426818580987651E-2</v>
+      </c>
+      <c r="C81">
+        <v>-8.7700109446845094E-4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2">
+        <v>35674</v>
+      </c>
+      <c r="B82">
+        <v>7.3925242571776881E-3</v>
+      </c>
+      <c r="C82">
+        <v>1.4361031209467589E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2">
+        <v>35704</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2">
+        <v>35735</v>
+      </c>
+      <c r="B84">
+        <v>2.8954097636229217E-3</v>
+      </c>
+      <c r="C84">
+        <v>2.8375176695209429E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2">
+        <v>35765</v>
+      </c>
+      <c r="B85">
+        <v>-1.4913344776148942E-2</v>
+      </c>
+      <c r="C85">
+        <v>9.0449512017683701E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2">
+        <v>35796</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2">
+        <v>35827</v>
+      </c>
+      <c r="B87">
+        <v>2.1929819961877699E-2</v>
+      </c>
+      <c r="C87">
+        <v>-1.1739313008827412E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2">
+        <v>35855</v>
+      </c>
+      <c r="B88">
+        <v>-7.0838478686310359E-5</v>
+      </c>
+      <c r="C88">
+        <v>1.1386099317234295E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2">
+        <v>35886</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2">
+        <v>35916</v>
+      </c>
+      <c r="B90">
+        <v>1.7119640618117004E-2</v>
+      </c>
+      <c r="C90">
+        <v>-9.2137151886763306E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2">
+        <v>35947</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2">
+        <v>35977</v>
+      </c>
+      <c r="B92">
+        <v>1.7197546783597615E-2</v>
+      </c>
+      <c r="C92">
+        <v>-5.822051343328024E-4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2">
+        <v>36008</v>
+      </c>
+      <c r="B93">
+        <v>1.3911820584860485E-2</v>
+      </c>
+      <c r="C93">
+        <v>8.0799934278300133E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="2">
+        <v>36039</v>
+      </c>
+      <c r="B94">
+        <v>4.9931036355358976E-2</v>
+      </c>
+      <c r="C94">
+        <v>1.1979250570806569E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="2">
+        <v>36069</v>
+      </c>
+      <c r="B95">
+        <v>-0.25722374927735275</v>
+      </c>
+      <c r="C95">
+        <v>7.7791307929680831E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2">
+        <v>36100</v>
+      </c>
+      <c r="B96">
+        <v>-1.1751409400982288E-2</v>
+      </c>
+      <c r="C96">
+        <v>-5.1449425988856086E-4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="2">
+        <v>36130</v>
+      </c>
+      <c r="B97">
+        <v>-6.5521075652324706E-2</v>
+      </c>
+      <c r="C97">
+        <v>1.2902908061856445E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="2">
+        <v>36161</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="2">
+        <v>36192</v>
+      </c>
+      <c r="B99">
+        <v>3.7490361020357653E-2</v>
+      </c>
+      <c r="C99">
+        <v>-3.7824548765446192E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="2">
+        <v>36220</v>
+      </c>
+      <c r="B100">
+        <v>-3.8183480391506118E-2</v>
+      </c>
+      <c r="C100">
+        <v>5.3704704268848829E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="2">
+        <v>36251</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="2">
+        <v>36281</v>
+      </c>
+      <c r="B102">
+        <v>6.5569549535242799E-2</v>
+      </c>
+      <c r="C102">
+        <v>7.4406096943808436E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="2">
+        <v>36312</v>
+      </c>
+      <c r="B103">
+        <v>-6.9985719892126833E-2</v>
+      </c>
+      <c r="C103">
+        <v>3.3963439959585704E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="2">
+        <v>36342</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="2">
+        <v>36373</v>
+      </c>
+      <c r="B105">
+        <v>-8.1839486594238019E-3</v>
+      </c>
+      <c r="C105">
+        <v>1.5856802030669845E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="2">
+        <v>36404</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="2">
+        <v>36434</v>
+      </c>
+      <c r="B107">
+        <v>2.5432788282364387E-2</v>
+      </c>
+      <c r="C107">
+        <v>1.3616586874400151E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="2">
+        <v>36465</v>
+      </c>
+      <c r="B108">
+        <v>8.4808786567382999E-2</v>
+      </c>
+      <c r="C108">
+        <v>8.6377524094366567E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="2">
+        <v>36495</v>
+      </c>
+      <c r="B109">
+        <v>-3.9452039946816404E-3</v>
+      </c>
+      <c r="C109">
+        <v>9.644129544541382E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="2">
+        <v>36526</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="2">
+        <v>36557</v>
+      </c>
+      <c r="B111">
+        <v>4.8797575946349231E-3</v>
+      </c>
+      <c r="C111">
+        <v>-3.2699731483576979E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="2">
+        <v>36586</v>
+      </c>
+      <c r="B112">
+        <v>-3.4829888225480735E-2</v>
+      </c>
+      <c r="C112">
+        <v>1.5624225361046958E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="2">
+        <v>36617</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="2">
+        <v>36647</v>
+      </c>
+      <c r="B114">
+        <v>4.5185932686871703E-2</v>
+      </c>
+      <c r="C114">
+        <v>7.108617884439567E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="2">
+        <v>36678</v>
+      </c>
+      <c r="B115">
+        <v>-1.6588958120098203E-2</v>
+      </c>
+      <c r="C115">
+        <v>-1.7442073030626698E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="2">
+        <v>36708</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="2">
+        <v>36739</v>
+      </c>
+      <c r="B117">
+        <v>1.1989009298383054E-2</v>
+      </c>
+      <c r="C117">
+        <v>-9.9187780112240283E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="2">
+        <v>36770</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2">
+        <v>36800</v>
+      </c>
+      <c r="B119">
+        <v>5.1987165584690229E-2</v>
+      </c>
+      <c r="C119">
+        <v>5.6066075659765343E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="2">
+        <v>36831</v>
+      </c>
+      <c r="B120">
+        <v>5.7625863535989835E-3</v>
+      </c>
+      <c r="C120">
+        <v>5.522706348879E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="2">
+        <v>36861</v>
+      </c>
+      <c r="B121">
+        <v>2.2349873796396528E-2</v>
+      </c>
+      <c r="C121">
+        <v>-1.1523859360593887E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="2">
+        <v>36892</v>
+      </c>
+      <c r="B122">
+        <v>-5.0739220075276335E-2</v>
+      </c>
+      <c r="C122">
+        <v>-4.5462144358119426E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="2">
+        <v>36923</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="2">
+        <v>36951</v>
+      </c>
+      <c r="B124">
+        <v>-5.5679468098602462E-2</v>
+      </c>
+      <c r="C124">
+        <v>2.9069051591354457E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="2">
+        <v>36982</v>
+      </c>
+      <c r="B125">
+        <v>-0.34226728035350346</v>
+      </c>
+      <c r="C125">
+        <v>-1.5946187112383922E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="2">
+        <v>37012</v>
+      </c>
+      <c r="B126">
+        <v>-0.11631059747443014</v>
+      </c>
+      <c r="C126">
+        <v>3.1691178857665807E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="2">
+        <v>37043</v>
+      </c>
+      <c r="B127">
+        <v>3.2558434669094E-2</v>
+      </c>
+      <c r="C127">
+        <v>-9.0146010390941764E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="2">
+        <v>37073</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="2">
+        <v>37104</v>
+      </c>
+      <c r="B129">
+        <v>4.831704048897497E-2</v>
+      </c>
+      <c r="C129">
+        <v>1.6211678472449371E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="2">
+        <v>37135</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="2">
+        <v>37165</v>
+      </c>
+      <c r="B131">
+        <v>4.0134459668364226E-4</v>
+      </c>
+      <c r="C131">
+        <v>-3.7589366977649877E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="2">
+        <v>37196</v>
+      </c>
+      <c r="B132">
+        <v>-1.2605960158113313E-2</v>
+      </c>
+      <c r="C132">
+        <v>-1.0083538298201616E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="2">
+        <v>37226</v>
+      </c>
+      <c r="B133">
+        <v>2.639194694583484E-2</v>
+      </c>
+      <c r="C133">
+        <v>7.7241831848258932E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="2">
+        <v>37257</v>
+      </c>
+      <c r="B134">
+        <v>2.0327770797694183E-2</v>
+      </c>
+      <c r="C134">
+        <v>2.3811288162530413E-2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="2">
+        <v>37288</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="2">
+        <v>37316</v>
+      </c>
+      <c r="B136">
+        <v>-2.854353272073451E-2</v>
+      </c>
+      <c r="C136">
+        <v>3.2674692852131676E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="2">
+        <v>37347</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="2">
+        <v>37377</v>
+      </c>
+      <c r="B138">
+        <v>1.8308638292936684E-2</v>
+      </c>
+      <c r="C138">
+        <v>-2.2777393676217159E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="2">
+        <v>37408</v>
+      </c>
+      <c r="B139">
+        <v>2.2907119002771759E-2</v>
+      </c>
+      <c r="C139">
+        <v>-9.1756635833481655E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="2">
+        <v>37438</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="2">
+        <v>37469</v>
+      </c>
+      <c r="B141">
+        <v>-3.1152544488063531E-2</v>
+      </c>
+      <c r="C141">
+        <v>1.5010354125580445E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="2">
+        <v>37500</v>
+      </c>
+      <c r="B142">
+        <v>-1.6977501097725448E-2</v>
+      </c>
+      <c r="C142">
+        <v>9.6462786709722199E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="2">
+        <v>37530</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="2">
+        <v>37561</v>
+      </c>
+      <c r="B144">
+        <v>-5.5909481916083317E-2</v>
+      </c>
+      <c r="C144">
+        <v>-2.0724770221827025E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="2">
+        <v>37591</v>
+      </c>
+      <c r="B145">
+        <v>3.182210862562098E-2</v>
+      </c>
+      <c r="C145">
+        <v>-4.5341254111285617E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="2">
+        <v>37622</v>
+      </c>
+      <c r="B146">
+        <v>3.1195721735109861E-2</v>
+      </c>
+      <c r="C146">
+        <v>3.1458586977572853E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="2">
+        <v>37653</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="2">
+        <v>37681</v>
+      </c>
+      <c r="B148">
+        <v>-2.4046125966334583E-3</v>
+      </c>
+      <c r="C148">
+        <v>-4.0770638097915755E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="2">
+        <v>37712</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="2">
+        <v>37742</v>
+      </c>
+      <c r="B150">
+        <v>-2.9159977514418164E-2</v>
+      </c>
+      <c r="C150">
+        <v>-5.390195392970509E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="2">
+        <v>37773</v>
+      </c>
+      <c r="B151">
+        <v>0.14826349896083099</v>
+      </c>
+      <c r="C151">
+        <v>-3.0148211131013642E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="2">
+        <v>37803</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="2">
+        <v>37834</v>
+      </c>
+      <c r="B153">
+        <v>2.4823486602164532E-2</v>
+      </c>
+      <c r="C153">
+        <v>2.6458367189849775E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="2">
+        <v>37865</v>
+      </c>
+      <c r="B154">
+        <v>-2.9631811802586776E-2</v>
+      </c>
+      <c r="C154">
+        <v>1.3333534254026586E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="2">
+        <v>37895</v>
+      </c>
+      <c r="B155">
+        <v>-5.4448713048491082E-4</v>
+      </c>
+      <c r="C155">
+        <v>-9.4210991562364132E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="2">
+        <v>37926</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="2">
+        <v>37956</v>
+      </c>
+      <c r="B157">
+        <v>5.5981506957009219E-3</v>
+      </c>
+      <c r="C157">
+        <v>9.2891352950293885E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="2">
+        <v>37987</v>
+      </c>
+      <c r="B158">
+        <v>-2.1050589992669448E-2</v>
+      </c>
+      <c r="C158">
+        <v>1.9372056076563646E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="2">
+        <v>38018</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="2">
+        <v>38047</v>
+      </c>
+      <c r="B160">
+        <v>-1.6483521979880341E-2</v>
+      </c>
+      <c r="C160">
+        <v>6.1209413609278332E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="2">
+        <v>38078</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="2">
+        <v>38108</v>
+      </c>
+      <c r="B162">
+        <v>-6.080926705658385E-4</v>
+      </c>
+      <c r="C162">
+        <v>1.2649029158960091E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="2">
+        <v>38139</v>
+      </c>
+      <c r="B163">
+        <v>-2.5950597301901582E-2</v>
+      </c>
+      <c r="C163">
+        <v>2.0909598170129929E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="2">
+        <v>38169</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="2">
+        <v>38200</v>
+      </c>
+      <c r="B165">
+        <v>9.191258402208257E-3</v>
+      </c>
+      <c r="C165">
+        <v>2.6464869814247886E-4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="2">
+        <v>38231</v>
+      </c>
+      <c r="B166">
+        <v>-7.5979603040983073E-3</v>
+      </c>
+      <c r="C166">
+        <v>-1.8276018397083529E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="2">
+        <v>38261</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="2">
+        <v>38292</v>
+      </c>
+      <c r="B168">
+        <v>1.3643392656268924E-2</v>
+      </c>
+      <c r="C168">
+        <v>4.593718720898407E-3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="2">
+        <v>38322</v>
+      </c>
+      <c r="B169">
+        <v>-1.7796567540248655E-3</v>
+      </c>
+      <c r="C169">
+        <v>8.6105242377515177E-3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="2">
+        <v>38353</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="2">
+        <v>38384</v>
+      </c>
+      <c r="B171">
+        <v>-5.335061089435887E-3</v>
+      </c>
+      <c r="C171">
+        <v>5.2768141878957852E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="2">
+        <v>38412</v>
+      </c>
+      <c r="B172">
+        <v>-1.1763995947313975E-2</v>
+      </c>
+      <c r="C172">
+        <v>1.7999376959092546E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="2">
+        <v>38443</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" s="2">
+        <v>38473</v>
+      </c>
+      <c r="B174">
+        <v>6.7792512900092501E-3</v>
+      </c>
+      <c r="C174">
+        <v>-4.8565449360102935E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="2">
+        <v>38504</v>
+      </c>
+      <c r="B175">
+        <v>2.274442795766406E-2</v>
+      </c>
+      <c r="C175">
+        <v>-5.6773612595095134E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="2">
+        <v>38534</v>
+      </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="2">
+        <v>38565</v>
+      </c>
+      <c r="B177">
+        <v>-1.460839706422206E-2</v>
+      </c>
+      <c r="C177">
+        <v>1.6666909024117757E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="2">
+        <v>38596</v>
+      </c>
+      <c r="B178">
+        <v>1.6638825525176332E-2</v>
+      </c>
+      <c r="C178">
+        <v>1.1227276193538221E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="2">
+        <v>38626</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="2">
+        <v>38657</v>
+      </c>
+      <c r="B180">
+        <v>3.5550426042323807E-3</v>
+      </c>
+      <c r="C180">
+        <v>-7.7381830881868268E-3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="2">
+        <v>38687</v>
+      </c>
+      <c r="B181">
+        <v>-1.8931020459149847E-3</v>
+      </c>
+      <c r="C181">
+        <v>-2.619613260986673E-3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="2">
+        <v>38718</v>
+      </c>
+      <c r="B182">
+        <v>1.2717154196954936E-2</v>
+      </c>
+      <c r="C182">
+        <v>1.3763655955745194E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="2">
+        <v>38749</v>
+      </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="2">
+        <v>38777</v>
+      </c>
+      <c r="B184">
+        <v>2.3698189287905687E-2</v>
+      </c>
+      <c r="C184">
+        <v>1.5120733893514232E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="2">
+        <v>38808</v>
+      </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="2">
+        <v>38838</v>
+      </c>
+      <c r="B186">
+        <v>5.1024509942111981E-2</v>
+      </c>
+      <c r="C186">
+        <v>-1.7664339639690805E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="2">
+        <v>38869</v>
+      </c>
+      <c r="B187">
+        <v>-6.2936845394398165E-3</v>
+      </c>
+      <c r="C187">
+        <v>-1.4970690177093614E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="2">
+        <v>38899</v>
+      </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="2">
+        <v>38930</v>
+      </c>
+      <c r="B189">
+        <v>-1.8125468466691975E-2</v>
+      </c>
+      <c r="C189">
+        <v>-1.625520196649851E-3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="2">
+        <v>38961</v>
+      </c>
+      <c r="B190">
+        <v>2.1826466568417746E-2</v>
+      </c>
+      <c r="C190">
+        <v>-2.0637525089782192E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="2">
+        <v>38991</v>
+      </c>
+      <c r="B191">
+        <v>-9.6522583923524599E-3</v>
+      </c>
+      <c r="C191">
+        <v>1.606961160882811E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="2">
+        <v>39022</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="2">
+        <v>39052</v>
+      </c>
+      <c r="B193">
+        <v>2.167291832155236E-2</v>
+      </c>
+      <c r="C193">
+        <v>-7.6039743471036873E-3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" s="2">
+        <v>39083</v>
+      </c>
+      <c r="B194">
+        <v>1.4602019446010608E-2</v>
+      </c>
+      <c r="C194">
+        <v>-7.7456672851275964E-3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="2">
+        <v>39114</v>
+      </c>
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="2">
+        <v>39142</v>
+      </c>
+      <c r="B196">
+        <v>3.5171447022849314E-3</v>
+      </c>
+      <c r="C196">
+        <v>-1.0270594481172832E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="2">
+        <v>39173</v>
+      </c>
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="2">
+        <v>39203</v>
+      </c>
+      <c r="B198">
+        <v>2.8806670176541017E-2</v>
+      </c>
+      <c r="C198">
+        <v>1.5193775776968024E-3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="2">
+        <v>39234</v>
+      </c>
+      <c r="B199">
+        <v>5.292622328994444E-3</v>
+      </c>
+      <c r="C199">
+        <v>-5.914948997449293E-4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="2">
+        <v>39264</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="2">
+        <v>39295</v>
+      </c>
+      <c r="B201">
+        <v>1.5306594614487235E-2</v>
+      </c>
+      <c r="C201">
+        <v>-1.5325075546418928E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="2">
+        <v>39326</v>
+      </c>
+      <c r="B202">
+        <v>-0.15087204695367681</v>
+      </c>
+      <c r="C202">
+        <v>2.5917635629851572E-3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="2">
+        <v>39356</v>
+      </c>
+      <c r="B203">
+        <v>5.1640063477094225E-2</v>
+      </c>
+      <c r="C203">
+        <v>6.5956866095979311E-3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="2">
+        <v>39387</v>
+      </c>
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="2">
+        <v>39417</v>
+      </c>
+      <c r="B205">
+        <v>8.5604771207966349E-2</v>
+      </c>
+      <c r="C205">
+        <v>-1.4489556709134564E-2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="2">
+        <v>39448</v>
+      </c>
+      <c r="B206">
+        <v>-0.17953813277030234</v>
+      </c>
+      <c r="C206">
+        <v>-4.3343705885406911E-2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="2">
+        <v>39479</v>
+      </c>
+      <c r="B207">
+        <v>0</v>
+      </c>
+      <c r="C207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="2">
+        <v>39508</v>
+      </c>
+      <c r="B208">
+        <v>0.19964587334006872</v>
+      </c>
+      <c r="C208">
+        <v>-3.4137136766124607E-2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="2">
+        <v>39539</v>
+      </c>
+      <c r="B209">
+        <v>-1.581746584646708E-3</v>
+      </c>
+      <c r="C209">
+        <v>-8.8810529813264337E-3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="2">
+        <v>39569</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="2">
+        <v>39600</v>
+      </c>
+      <c r="B211">
+        <v>5.6705520555498101E-3</v>
+      </c>
+      <c r="C211">
+        <v>1.1143756349928634E-2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="2">
+        <v>39630</v>
+      </c>
+      <c r="B212">
+        <v>0</v>
+      </c>
+      <c r="C212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="2">
+        <v>39661</v>
+      </c>
+      <c r="B213">
+        <v>2.6696412194356658E-2</v>
+      </c>
+      <c r="C213">
+        <v>-6.4689530669122842E-3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" s="2">
+        <v>39692</v>
+      </c>
+      <c r="B214">
+        <v>0.13209147713228855</v>
+      </c>
+      <c r="C214">
+        <v>-2.6264461450677783E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" s="2">
+        <v>39722</v>
+      </c>
+      <c r="B215">
+        <v>-3.1765068720527229E-2</v>
+      </c>
+      <c r="C215">
+        <v>-7.2139619624682488E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="2">
+        <v>39753</v>
+      </c>
+      <c r="B216">
+        <v>6.0893088074141399E-2</v>
+      </c>
+      <c r="C216">
+        <v>-2.9376884367625644E-3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="2">
+        <v>39783</v>
+      </c>
+      <c r="B217">
+        <v>-2.8391905082123886E-2</v>
+      </c>
+      <c r="C217">
+        <v>-8.9372096899050638E-2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="2">
+        <v>39814</v>
+      </c>
+      <c r="B218">
+        <v>3.0782171041503936E-2</v>
+      </c>
+      <c r="C218">
+        <v>1.8993892689203318E-2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="2">
+        <v>39845</v>
+      </c>
+      <c r="B219">
+        <v>0</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="2">
+        <v>39873</v>
+      </c>
+      <c r="B220">
+        <v>6.8719924587034853E-2</v>
+      </c>
+      <c r="C220">
+        <v>-2.4167234319684039E-2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="2">
+        <v>39904</v>
+      </c>
+      <c r="B221">
+        <v>-7.5249767404802353E-4</v>
+      </c>
+      <c r="C221">
+        <v>2.3008510489476146E-3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="2">
+        <v>39934</v>
+      </c>
+      <c r="B222">
+        <v>0</v>
+      </c>
+      <c r="C222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="2">
+        <v>39965</v>
+      </c>
+      <c r="B223">
+        <v>1.1927061488920599E-2</v>
+      </c>
+      <c r="C223">
+        <v>-2.911619867610668E-3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="2">
+        <v>39995</v>
+      </c>
+      <c r="B224">
+        <v>0</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" s="2">
+        <v>40026</v>
+      </c>
+      <c r="B225">
+        <v>1.7190414824253028E-2</v>
+      </c>
+      <c r="C225">
+        <v>1.1243903232220669E-2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="2">
+        <v>40057</v>
+      </c>
+      <c r="B226">
+        <v>-1.8798799419664624E-2</v>
+      </c>
+      <c r="C226">
+        <v>1.5470102632700728E-2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" s="2">
+        <v>40087</v>
+      </c>
+      <c r="B227">
+        <v>0</v>
+      </c>
+      <c r="C227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" s="2">
+        <v>40118</v>
+      </c>
+      <c r="B228">
+        <v>-3.1359250052684896E-2</v>
+      </c>
+      <c r="C228">
+        <v>1.0391451157228018E-2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" s="2">
+        <v>40148</v>
+      </c>
+      <c r="B229">
+        <v>-2.5728699544006702E-2</v>
+      </c>
+      <c r="C229">
+        <v>3.119640217421954E-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="2">
+        <v>40179</v>
+      </c>
+      <c r="B230">
+        <v>1.266283139656716E-2</v>
+      </c>
+      <c r="C230">
+        <v>-7.2772972864780325E-3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="2">
+        <v>40210</v>
+      </c>
+      <c r="B231">
+        <v>0</v>
+      </c>
+      <c r="C231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="2">
+        <v>40238</v>
+      </c>
+      <c r="B232">
+        <v>-1.7545373528153042E-2</v>
+      </c>
+      <c r="C232">
+        <v>-6.0490502528260347E-3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="2">
+        <v>40269</v>
+      </c>
+      <c r="B233">
+        <v>-1.5896527151241065E-2</v>
+      </c>
+      <c r="C233">
+        <v>1.8875525697296124E-2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="2">
+        <v>40299</v>
+      </c>
+      <c r="B234">
+        <v>0</v>
+      </c>
+      <c r="C234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="2">
+        <v>40330</v>
+      </c>
+      <c r="B235">
+        <v>2.011664487492004E-3</v>
+      </c>
+      <c r="C235">
+        <v>-6.6250664856852236E-3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="2">
+        <v>40360</v>
+      </c>
+      <c r="B236">
+        <v>0</v>
+      </c>
+      <c r="C236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="2">
+        <v>40391</v>
+      </c>
+      <c r="B237">
+        <v>-5.0776818367207288E-3</v>
+      </c>
+      <c r="C237">
+        <v>4.949362384463819E-3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="2">
+        <v>40422</v>
+      </c>
+      <c r="B238">
+        <v>-8.0253675115476986E-3</v>
+      </c>
+      <c r="C238">
+        <v>-1.3258003476793385E-2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="2">
+        <v>40452</v>
+      </c>
+      <c r="B239">
+        <v>0</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="2">
+        <v>40483</v>
+      </c>
+      <c r="B240">
+        <v>-1.3729402276887348E-2</v>
+      </c>
+      <c r="C240">
+        <v>1.1033337635436184E-2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="2">
+        <v>40513</v>
+      </c>
+      <c r="B241">
+        <v>2.0536525253206511E-3</v>
+      </c>
+      <c r="C241">
+        <v>-2.3580275487262051E-3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="2">
+        <v>40544</v>
+      </c>
+      <c r="B242">
+        <v>-2.8400212523943057E-2</v>
+      </c>
+      <c r="C242">
+        <v>1.2358602105593967E-2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="2">
+        <v>40575</v>
+      </c>
+      <c r="B243">
+        <v>0</v>
+      </c>
+      <c r="C243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" s="2">
+        <v>40603</v>
+      </c>
+      <c r="B244">
+        <v>-1.6502122553883097E-2</v>
+      </c>
+      <c r="C244">
+        <v>7.7641325260792192E-3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="2">
+        <v>40634</v>
+      </c>
+      <c r="B245">
+        <v>-1.3456067779050495E-2</v>
+      </c>
+      <c r="C245">
+        <v>2.4299962012304843E-3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="2">
+        <v>40664</v>
+      </c>
+      <c r="B246">
+        <v>0</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="2">
+        <v>40695</v>
+      </c>
+      <c r="B247">
+        <v>-3.5328069968899563E-3</v>
+      </c>
+      <c r="C247">
+        <v>-1.1022361729955868E-2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="2">
+        <v>40725</v>
+      </c>
+      <c r="B248">
+        <v>0</v>
+      </c>
+      <c r="C248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="2">
+        <v>40756</v>
+      </c>
+      <c r="B249">
+        <v>1.1446364286270379E-2</v>
+      </c>
+      <c r="C249">
+        <v>7.2276764074093534E-3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" s="2">
+        <v>40787</v>
+      </c>
+      <c r="B250">
+        <v>1.4968962623641377E-2</v>
+      </c>
+      <c r="C250">
+        <v>1.8374116511100155E-3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" s="2">
+        <v>40817</v>
+      </c>
+      <c r="B251">
+        <v>0</v>
+      </c>
+      <c r="C251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="2">
+        <v>40848</v>
+      </c>
+      <c r="B252">
+        <v>-5.108727537498501E-3</v>
+      </c>
+      <c r="C252">
+        <v>-4.2288434284611549E-3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="2">
+        <v>40878</v>
+      </c>
+      <c r="B253">
+        <v>-2.8288292534925902E-2</v>
+      </c>
+      <c r="C253">
+        <v>4.5118558406127543E-3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="2">
+        <v>40909</v>
+      </c>
+      <c r="B254">
+        <v>1.012545329855067E-2</v>
+      </c>
+      <c r="C254">
+        <v>-5.8512128763393567E-3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" s="2">
+        <v>40940</v>
+      </c>
+      <c r="B255">
+        <v>0</v>
+      </c>
+      <c r="C255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" s="2">
+        <v>40969</v>
+      </c>
+      <c r="B256">
+        <v>8.2667113606917503E-3</v>
+      </c>
+      <c r="C256">
+        <v>-2.4875705998783932E-3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="2">
+        <v>41000</v>
+      </c>
+      <c r="B257">
+        <v>1.7450059584895549E-2</v>
+      </c>
+      <c r="C257">
+        <v>-9.6184159989500233E-3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" s="2">
+        <v>41030</v>
+      </c>
+      <c r="B258">
+        <v>0</v>
+      </c>
+      <c r="C258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" s="2">
+        <v>41061</v>
+      </c>
+      <c r="B259">
+        <v>1.632525390287299E-2</v>
+      </c>
+      <c r="C259">
+        <v>1.067322128692743E-4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="2">
+        <v>41091</v>
+      </c>
+      <c r="B260">
+        <v>0</v>
+      </c>
+      <c r="C260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="2">
+        <v>41122</v>
+      </c>
+      <c r="B261">
+        <v>1.8199479295240881E-2</v>
+      </c>
+      <c r="C261">
+        <v>1.6760405256282824E-3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="2">
+        <v>41153</v>
+      </c>
+      <c r="B262">
+        <v>3.1165478867403298E-2</v>
+      </c>
+      <c r="C262">
+        <v>-1.6002944410706592E-2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" s="2">
+        <v>41183</v>
+      </c>
+      <c r="B263">
+        <v>1.7306969016722629E-2</v>
+      </c>
+      <c r="C263">
+        <v>-7.6523137283001502E-4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="2">
+        <v>41214</v>
+      </c>
+      <c r="B264">
+        <v>0</v>
+      </c>
+      <c r="C264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" s="2">
+        <v>41244</v>
+      </c>
+      <c r="B265">
+        <v>1.6847081559497944E-2</v>
+      </c>
+      <c r="C265">
+        <v>-1.4790803549105523E-2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" s="2">
+        <v>41275</v>
+      </c>
+      <c r="B266">
+        <v>1.196472372760558E-2</v>
+      </c>
+      <c r="C266">
+        <v>1.5373857166906325E-2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" s="2">
+        <v>41306</v>
+      </c>
+      <c r="B267">
+        <v>0</v>
+      </c>
+      <c r="C267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="2">
+        <v>41334</v>
+      </c>
+      <c r="B268">
+        <v>2.8857075618044646E-2</v>
+      </c>
+      <c r="C268">
+        <v>4.3948634418423307E-3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" s="2">
+        <v>41365</v>
+      </c>
+      <c r="B269">
+        <v>0</v>
+      </c>
+      <c r="C269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" s="2">
+        <v>41395</v>
+      </c>
+      <c r="B270">
+        <v>3.0577250882409045E-2</v>
+      </c>
+      <c r="C270">
+        <v>-1.1816003866019439E-2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" s="2">
+        <v>41426</v>
+      </c>
+      <c r="B271">
+        <v>1.8295600726261699E-2</v>
+      </c>
+      <c r="C271">
+        <v>-4.3297490573500474E-3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" s="2">
+        <v>41456</v>
+      </c>
+      <c r="B272">
+        <v>2.9465401738224426E-3</v>
+      </c>
+      <c r="C272">
+        <v>2.0522289647506228E-2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" s="2">
+        <v>41487</v>
+      </c>
+      <c r="B273">
+        <v>0</v>
+      </c>
+      <c r="C273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" s="2">
+        <v>41518</v>
+      </c>
+      <c r="B274">
+        <v>1.7960913198555115E-2</v>
+      </c>
+      <c r="C274">
+        <v>-1.1344474423705323E-2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" s="2">
+        <v>41548</v>
+      </c>
+      <c r="B275">
+        <v>-5.6935556999494351E-4</v>
+      </c>
+      <c r="C275">
+        <v>-8.9888471582465559E-5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="2">
+        <v>41579</v>
+      </c>
+      <c r="B276">
+        <v>0</v>
+      </c>
+      <c r="C276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" s="2">
+        <v>41609</v>
+      </c>
+      <c r="B277">
+        <v>1.7469244519432665E-2</v>
+      </c>
+      <c r="C277">
+        <v>-5.3959371139034804E-3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="2">
+        <v>41640</v>
+      </c>
+      <c r="B278">
+        <v>2.6406564717576329E-2</v>
+      </c>
+      <c r="C278">
+        <v>5.5090017085808749E-3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" s="2">
+        <v>41671</v>
+      </c>
+      <c r="B279">
+        <v>0</v>
+      </c>
+      <c r="C279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" s="2">
+        <v>41699</v>
+      </c>
+      <c r="B280">
+        <v>2.0754526532998935E-3</v>
+      </c>
+      <c r="C280">
+        <v>-8.779162579987114E-3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" s="2">
+        <v>41730</v>
+      </c>
+      <c r="B281">
+        <v>-1.2938531408450148E-2</v>
+      </c>
+      <c r="C281">
+        <v>1.7884101574672271E-2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" s="2">
+        <v>41760</v>
+      </c>
+      <c r="B282">
+        <v>0</v>
+      </c>
+      <c r="C282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" s="2">
+        <v>41791</v>
+      </c>
+      <c r="B283">
+        <v>-6.6964947152988504E-3</v>
+      </c>
+      <c r="C283">
+        <v>1.7480030908143037E-2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" s="2">
+        <v>41821</v>
+      </c>
+      <c r="B284">
+        <v>-5.7028998212782026E-3</v>
+      </c>
+      <c r="C284">
+        <v>-7.2946884658241142E-4</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" s="2">
+        <v>41852</v>
+      </c>
+      <c r="B285">
+        <v>0</v>
+      </c>
+      <c r="C285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" s="2">
+        <v>41883</v>
+      </c>
+      <c r="B286">
+        <v>1.0813822131950793E-2</v>
+      </c>
+      <c r="C286">
+        <v>-9.7983479027852621E-3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" s="2">
+        <v>41913</v>
+      </c>
+      <c r="B287">
+        <v>2.3509187378645054E-2</v>
+      </c>
+      <c r="C287">
+        <v>3.1599252502049029E-3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" s="2">
+        <v>41944</v>
+      </c>
+      <c r="B288">
+        <v>0</v>
+      </c>
+      <c r="C288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" s="2">
+        <v>41974</v>
+      </c>
+      <c r="B289">
+        <v>1.7783597030490293E-2</v>
+      </c>
+      <c r="C289">
+        <v>-3.4985289746086862E-3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" s="2">
+        <v>42005</v>
+      </c>
+      <c r="B290">
+        <v>1.1106028972803718E-2</v>
+      </c>
+      <c r="C290">
+        <v>2.4517735903991757E-3</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B291">
+        <v>0</v>
+      </c>
+      <c r="C291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" s="2">
+        <v>42064</v>
+      </c>
+      <c r="B292">
+        <v>-1.2614939548448494E-2</v>
+      </c>
+      <c r="C292">
+        <v>9.6647706799343133E-3</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" s="2">
+        <v>42095</v>
+      </c>
+      <c r="B293">
+        <v>-3.7933734801115131E-3</v>
+      </c>
+      <c r="C293">
+        <v>2.4966795345105308E-3</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" s="2">
+        <v>42125</v>
+      </c>
+      <c r="B294">
+        <v>0</v>
+      </c>
+      <c r="C294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" s="2">
+        <v>42156</v>
+      </c>
+      <c r="B295">
+        <v>5.7364297615681414E-3</v>
+      </c>
+      <c r="C295">
+        <v>2.359925658260128E-3</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" s="2">
+        <v>42186</v>
+      </c>
+      <c r="B296">
+        <v>1.0695684864653767E-2</v>
+      </c>
+      <c r="C296">
+        <v>-1.3030107834668641E-2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" s="2">
+        <v>42217</v>
+      </c>
+      <c r="B297">
+        <v>0</v>
+      </c>
+      <c r="C297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" s="2">
+        <v>42248</v>
+      </c>
+      <c r="B298">
+        <v>-3.1845965145346877E-2</v>
+      </c>
+      <c r="C298">
+        <v>-7.8724369067358288E-3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299" s="2">
+        <v>42278</v>
+      </c>
+      <c r="B299">
+        <v>4.735916964100071E-2</v>
+      </c>
+      <c r="C299">
+        <v>7.9760798324943968E-3</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="A300" s="2">
+        <v>42309</v>
+      </c>
+      <c r="B300">
+        <v>0</v>
+      </c>
+      <c r="C300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301" s="2">
+        <v>42339</v>
+      </c>
+      <c r="B301">
+        <v>3.7165902784518819E-2</v>
+      </c>
+      <c r="C301">
+        <v>-3.0881680856427686E-3</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" s="2">
+        <v>42370</v>
+      </c>
+      <c r="B302">
+        <v>4.9961332842437239E-3</v>
+      </c>
+      <c r="C302">
+        <v>-8.2441176984130241E-4</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303" s="2">
+        <v>42401</v>
+      </c>
+      <c r="B303">
+        <v>0</v>
+      </c>
+      <c r="C303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="A304" s="2">
+        <v>42430</v>
+      </c>
+      <c r="B304">
+        <v>-3.1574926937280826E-2</v>
+      </c>
+      <c r="C304">
+        <v>1.4573719753210881E-2</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
+      <c r="A305" s="2">
+        <v>42461</v>
+      </c>
+      <c r="B305">
+        <v>1.1886519078241528E-2</v>
+      </c>
+      <c r="C305">
+        <v>2.742289326711183E-3</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306" s="2">
+        <v>42491</v>
+      </c>
+      <c r="B306">
+        <v>0</v>
+      </c>
+      <c r="C306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="A307" s="2">
+        <v>42522</v>
+      </c>
+      <c r="B307">
+        <v>-1.8184765008654763E-2</v>
+      </c>
+      <c r="C307">
+        <v>7.324858728586175E-3</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3">
+      <c r="A308" s="2">
+        <v>42552</v>
+      </c>
+      <c r="B308">
+        <v>2.3304387296466068E-3</v>
+      </c>
+      <c r="C308">
+        <v>5.0775283723974865E-4</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3">
+      <c r="A309" s="2">
+        <v>42583</v>
+      </c>
+      <c r="B309">
+        <v>0</v>
+      </c>
+      <c r="C309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3">
+      <c r="A310" s="2">
+        <v>42614</v>
+      </c>
+      <c r="B310">
+        <v>-1.0994950853533013E-2</v>
+      </c>
+      <c r="C310">
+        <v>1.1878516891296346E-2</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3">
+      <c r="A311" s="2">
+        <v>42644</v>
+      </c>
+      <c r="B311">
+        <v>0</v>
+      </c>
+      <c r="C311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3">
+      <c r="A312" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B312">
+        <v>-3.6493778454582074E-3</v>
+      </c>
+      <c r="C312">
+        <v>-3.4572595391497425E-3</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3">
+      <c r="A313" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B313">
+        <v>2.5926982954344868E-2</v>
+      </c>
+      <c r="C313">
+        <v>-5.9522458154014982E-3</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3">
+      <c r="A314" s="2">
+        <v>42736</v>
+      </c>
+      <c r="B314">
+        <v>0</v>
+      </c>
+      <c r="C314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3">
+      <c r="A315" s="2">
+        <v>42767</v>
+      </c>
+      <c r="B315">
+        <v>4.375765751662839E-3</v>
+      </c>
+      <c r="C315">
+        <v>-2.6062562238225815E-3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3">
+      <c r="A316" s="2">
+        <v>42795</v>
+      </c>
+      <c r="B316">
+        <v>-2.0294757055467613E-2</v>
+      </c>
+      <c r="C316">
+        <v>-7.7567102890556371E-3</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3">
+      <c r="A317" s="2">
+        <v>42826</v>
+      </c>
+      <c r="B317">
+        <v>0</v>
+      </c>
+      <c r="C317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3">
+      <c r="A318" s="2">
+        <v>42856</v>
+      </c>
+      <c r="B318">
+        <v>1.4011460479045459E-2</v>
+      </c>
+      <c r="C318">
+        <v>9.6445589671653037E-3</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3">
+      <c r="A319" s="2">
+        <v>42887</v>
+      </c>
+      <c r="B319">
+        <v>2.1232594348040194E-2</v>
+      </c>
+      <c r="C319">
+        <v>2.7728822852802521E-3</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3">
+      <c r="A320" s="2">
+        <v>42917</v>
+      </c>
+      <c r="B320">
+        <v>-2.5433681535793227E-3</v>
+      </c>
+      <c r="C320">
+        <v>9.881983213073783E-4</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3">
+      <c r="A321" s="2">
+        <v>42948</v>
+      </c>
+      <c r="B321">
+        <v>0</v>
+      </c>
+      <c r="C321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3">
+      <c r="A322" s="2">
+        <v>42979</v>
+      </c>
+      <c r="B322">
+        <v>3.2954944861067592E-2</v>
+      </c>
+      <c r="C322">
+        <v>7.3791287486041903E-3</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3">
+      <c r="A323" s="2">
+        <v>43009</v>
+      </c>
+      <c r="B323">
+        <v>0</v>
+      </c>
+      <c r="C323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3">
+      <c r="A324" s="2">
+        <v>43040</v>
+      </c>
+      <c r="B324">
+        <v>5.9067102951102105E-3</v>
+      </c>
+      <c r="C324">
+        <v>8.9134690114158407E-3</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3">
+      <c r="A325" s="2">
+        <v>43070</v>
+      </c>
+      <c r="B325">
+        <v>6.0720404804843128E-3</v>
+      </c>
+      <c r="C325">
+        <v>-5.9145579414632858E-3</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3">
+      <c r="A326" s="2">
+        <v>43101</v>
+      </c>
+      <c r="B326">
+        <v>2.0315294043057569E-2</v>
+      </c>
+      <c r="C326">
+        <v>-6.161261494458494E-4</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3">
+      <c r="A327" s="2">
+        <v>43132</v>
+      </c>
+      <c r="B327">
+        <v>0</v>
+      </c>
+      <c r="C327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3">
+      <c r="A328" s="2">
+        <v>43160</v>
+      </c>
+      <c r="B328">
+        <v>1.0838746749187618E-2</v>
+      </c>
+      <c r="C328">
+        <v>-2.2634023325905275E-3</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3">
+      <c r="A329" s="2">
+        <v>43191</v>
+      </c>
+      <c r="B329">
+        <v>0</v>
+      </c>
+      <c r="C329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3">
+      <c r="A330" s="2">
+        <v>43221</v>
+      </c>
+      <c r="B330">
+        <v>8.849094054940481E-3</v>
+      </c>
+      <c r="C330">
+        <v>7.3293136946703027E-3</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3">
+      <c r="A331" s="2">
+        <v>43252</v>
+      </c>
+      <c r="B331">
+        <v>-4.1496113124037488E-3</v>
+      </c>
+      <c r="C331">
+        <v>1.0007235120533715E-2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3">
+      <c r="A332" s="2">
+        <v>43282</v>
+      </c>
+      <c r="B332">
+        <v>0</v>
+      </c>
+      <c r="C332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3">
+      <c r="A333" s="2">
+        <v>43313</v>
+      </c>
+      <c r="B333">
+        <v>1.3925877957963052E-2</v>
+      </c>
+      <c r="C333">
+        <v>-1.4976331063980755E-2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3">
+      <c r="A334" s="2">
+        <v>43344</v>
+      </c>
+      <c r="B334">
+        <v>2.3261115342347951E-2</v>
+      </c>
+      <c r="C334">
+        <v>-1.5871744510006936E-3</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3">
+      <c r="A335" s="2">
+        <v>43374</v>
+      </c>
+      <c r="B335">
+        <v>0</v>
+      </c>
+      <c r="C335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3">
+      <c r="A336" s="2">
+        <v>43405</v>
+      </c>
+      <c r="B336">
+        <v>6.5740275575984315E-3</v>
+      </c>
+      <c r="C336">
+        <v>4.8318013641977494E-3</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3">
+      <c r="A337" s="2">
+        <v>43435</v>
+      </c>
+      <c r="B337">
+        <v>2.6090804005388962E-2</v>
+      </c>
+      <c r="C337">
+        <v>-6.5709183031772266E-3</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="A338" s="2">
+        <v>43466</v>
+      </c>
+      <c r="B338">
+        <v>8.1578671990376224E-3</v>
+      </c>
+      <c r="C338">
+        <v>-2.4216579448346816E-3</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3">
+      <c r="A339" s="2">
+        <v>43497</v>
+      </c>
+      <c r="B339">
+        <v>0</v>
+      </c>
+      <c r="C339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3">
+      <c r="A340" s="2">
+        <v>43525</v>
+      </c>
+      <c r="B340">
+        <v>5.6171156009990932E-3</v>
+      </c>
+      <c r="C340">
+        <v>-3.0887059003750703E-3</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3">
+      <c r="A341" s="2">
+        <v>43556</v>
+      </c>
+      <c r="B341">
+        <v>0</v>
+      </c>
+      <c r="C341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3">
+      <c r="A342" s="2">
+        <v>43586</v>
+      </c>
+      <c r="B342">
+        <v>-2.0176493861809013E-2</v>
+      </c>
+      <c r="C342">
+        <v>3.7536990400079484E-3</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3">
+      <c r="A343" s="2">
+        <v>43617</v>
+      </c>
+      <c r="B343">
+        <v>-2.235390100940967E-2</v>
+      </c>
+      <c r="C343">
+        <v>-1.3329658734410301E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C337"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>33239</v>
       </c>

</xml_diff>